<commit_message>
die service trips are within travel time limits klopt dus ook niet
</commit_message>
<xml_diff>
--- a/Fault excel.xlsx
+++ b/Fault excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Youpk\Desktop\Toegepaste wiskunde\jaar 2\Project\Periode 1\Project 5\Visual Code Mapje\Project5_Team1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89475AEA-D3B9-4B5A-9A38-3A00A2F9D316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283D035F-67DE-4EA7-BDF6-85B7120B7AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="13770" xr2:uid="{3E87C0C4-D23B-4DB7-9B3E-4E14F9D15707}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
   <si>
     <t>startlocatie</t>
   </si>
@@ -520,7 +520,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -678,8 +678,8 @@
       <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
-        <v>20</v>
+      <c r="E5" s="3">
+        <v>0.2638888888888889</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>
@@ -908,6 +908,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002E31C4A0CECB6A45A7FD454675B3B06E" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="1c5a02c4a7b9916c860052fd492f2fca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3812522d-e2eb-474d-9675-21e7862faf23" xmlns:ns4="470a7cab-7f68-4375-affc-6f25e6cba559" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f85d6c68ced2529f1b9c0ba0e9cafd51" ns3:_="" ns4:_="">
     <xsd:import namespace="3812522d-e2eb-474d-9675-21e7862faf23"/>
@@ -1126,15 +1135,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1144,6 +1144,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E9428D1-86E1-476A-B227-3C2079B7F454}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{487F3C48-3814-460B-BDA7-6800B4D0EA03}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1158,14 +1166,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E9428D1-86E1-476A-B227-3C2079B7F454}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>